<commit_message>
Enemies now walk down the center of the path.
</commit_message>
<xml_diff>
--- a/PA9_Group2/Resources/pathDiagram.xlsx
+++ b/PA9_Group2/Resources/pathDiagram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\Drive Sync\CS_122\PA9\PA9_Group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\Drive Sync\CS_122\PA9\PA9_Group2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC86F71A-27B8-4C51-9F56-6F1AD1632FB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F09E03-2771-446D-983F-5393AACD79C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34F59E2-5A31-4EFD-B857-CFFB0A75CDB7}"/>
   </bookViews>
@@ -20277,6 +20277,156 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15601950" y="2476500"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="412" name="Picture 411">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{744EE99F-045A-407E-AAD5-240E2F4F9F82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13620750" y="3467100"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="414" name="Picture 413">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEE72EDC-B7BC-4188-BACF-6B91837BF27B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13620750" y="1733550"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="427" name="Picture 426">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B9D33E-8FC4-40B2-89DF-C89B5AFCB3D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11639550" y="3467100"/>
           <a:ext cx="256032" cy="256032"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20589,7 +20739,7 @@
   <dimension ref="R4:BK25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="BR10" sqref="BR10"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Grass backgrounds for textures, and fewer unnecessary outputs
</commit_message>
<xml_diff>
--- a/PA9_Group2/Resources/pathDiagram.xlsx
+++ b/PA9_Group2/Resources/pathDiagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\Drive Sync\CS_122\PA9\PA9_Group2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F09E03-2771-446D-983F-5393AACD79C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77986017-1A5E-48F5-852D-7EAA43297227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34F59E2-5A31-4EFD-B857-CFFB0A75CDB7}"/>
   </bookViews>
@@ -20188,6 +20188,306 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="452" name="Picture 451">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CAD5853-C377-4C58-BD53-6648988B1FAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15601950" y="2476500"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="412" name="Picture 411">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{744EE99F-045A-407E-AAD5-240E2F4F9F82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13620750" y="3467100"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="414" name="Picture 413">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEE72EDC-B7BC-4188-BACF-6B91837BF27B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13620750" y="1733550"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>8382</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>8382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="427" name="Picture 426">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B9D33E-8FC4-40B2-89DF-C89B5AFCB3D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11639550" y="3467100"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>236982</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>17907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D41690AA-89AD-4708-A965-224FFE7FCF1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15830550" y="2238375"/>
+          <a:ext cx="256032" cy="256032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="454" name="Picture 453">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19AE891E-93C9-4DA2-94EE-4D6060ABC54F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10648950" y="5200650"/>
+          <a:ext cx="247650" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
@@ -20201,19 +20501,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="450" name="Picture 449">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A149B7-4FBE-43BB-8954-C1B648AEF1CB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <xdr:cNvPr id="455" name="Picture 454">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F17BC179-863E-463D-AE13-90D8D85A1B9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -20227,206 +20527,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10648950" y="5200650"/>
-          <a:ext cx="256032" cy="256032"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>8382</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>8382</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="452" name="Picture 451">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CAD5853-C377-4C58-BD53-6648988B1FAB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15601950" y="2476500"/>
-          <a:ext cx="256032" cy="256032"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>8382</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>8382</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="412" name="Picture 411">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{744EE99F-045A-407E-AAD5-240E2F4F9F82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13620750" y="3467100"/>
-          <a:ext cx="256032" cy="256032"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>8382</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>8382</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="414" name="Picture 413">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEE72EDC-B7BC-4188-BACF-6B91837BF27B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13620750" y="1733550"/>
-          <a:ext cx="256032" cy="256032"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>8382</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>8382</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="427" name="Picture 426">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B9D33E-8FC4-40B2-89DF-C89B5AFCB3D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11639550" y="3467100"/>
           <a:ext cx="256032" cy="256032"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20739,7 +20839,7 @@
   <dimension ref="R4:BK25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="BP19" sqref="BP19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>